<commit_message>
ENDgit add --allgit add --allgit add --allgit add --allgit add --all
</commit_message>
<xml_diff>
--- a/Interpreter/Interpreter/Лист Microsoft Excel.xlsx
+++ b/Interpreter/Interpreter/Лист Microsoft Excel.xlsx
@@ -19,10 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="77">
-  <si>
-    <t>0,P6</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="103">
   <si>
     <t>F</t>
   </si>
@@ -78,9 +75,6 @@
     <t>11 (разделитель)</t>
   </si>
   <si>
-    <t>операторы</t>
-  </si>
-  <si>
     <t>=</t>
   </si>
   <si>
@@ -105,12 +99,6 @@
     <t xml:space="preserve">() {} [ ] </t>
   </si>
   <si>
-    <t>Z</t>
-  </si>
-  <si>
-    <t>8,P2</t>
-  </si>
-  <si>
     <t>p1 - identity</t>
   </si>
   <si>
@@ -135,21 +123,12 @@
     <t>p8 - clear cash</t>
   </si>
   <si>
-    <t>8,P3</t>
-  </si>
-  <si>
     <t>11,P3</t>
   </si>
   <si>
     <t>11, P2</t>
   </si>
   <si>
-    <t>10,P3</t>
-  </si>
-  <si>
-    <t>3,P3</t>
-  </si>
-  <si>
     <t>1,P5</t>
   </si>
   <si>
@@ -162,9 +141,6 @@
     <t>9,P5</t>
   </si>
   <si>
-    <t>10,P5</t>
-  </si>
-  <si>
     <t>11,P5</t>
   </si>
   <si>
@@ -243,20 +219,112 @@
     <t>15,P3</t>
   </si>
   <si>
+    <t>ab23,2684:of[1..3,10..20] of integer;</t>
+  </si>
+  <si>
+    <t>a:=321;</t>
+  </si>
+  <si>
+    <t>b&gt;a</t>
+  </si>
+  <si>
+    <t>b&lt;&gt;a</t>
+  </si>
+  <si>
+    <t>a := 'ssssss'</t>
+  </si>
+  <si>
+    <t>b = (a+z-215)</t>
+  </si>
+  <si>
+    <t>g = 0,015e1</t>
+  </si>
+  <si>
+    <t>12,P3</t>
+  </si>
+  <si>
+    <t>12,P2</t>
+  </si>
+  <si>
+    <t>13,P2</t>
+  </si>
+  <si>
+    <t>13,P3</t>
+  </si>
+  <si>
+    <t>операция +-</t>
+  </si>
+  <si>
+    <t>7,P2</t>
+  </si>
+  <si>
+    <t>7,P3</t>
+  </si>
+  <si>
+    <t>0,P2</t>
+  </si>
+  <si>
+    <t>15,P2</t>
+  </si>
+  <si>
+    <t>else</t>
+  </si>
+  <si>
+    <t>x1</t>
+  </si>
+  <si>
+    <t>0,P3</t>
+  </si>
+  <si>
+    <t>4,P5</t>
+  </si>
+  <si>
+    <t>4,P4</t>
+  </si>
+  <si>
+    <t>12,P4</t>
+  </si>
+  <si>
+    <t>13,P4</t>
+  </si>
+  <si>
+    <t>7,P4</t>
+  </si>
+  <si>
+    <t>9,P4</t>
+  </si>
+  <si>
+    <t>16(/)</t>
+  </si>
+  <si>
+    <t>16,P2</t>
+  </si>
+  <si>
+    <t>16,P3</t>
+  </si>
+  <si>
+    <t>16,P4</t>
+  </si>
+  <si>
+    <t>a:='ssssss';</t>
+  </si>
+  <si>
+    <t>g = 0,015e1;</t>
+  </si>
+  <si>
     <r>
-      <t>a,ba,c4s : array of [1..3</t>
+      <t>b&gt;</t>
     </r>
     <r>
       <rPr>
-        <b/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">, </t>
+      <t>a</t>
     </r>
     <r>
       <rPr>
@@ -266,19 +334,23 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>10..20</t>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>b&lt;&gt;</t>
     </r>
     <r>
       <rPr>
-        <b/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>]</t>
+      <t>a</t>
     </r>
     <r>
       <rPr>
@@ -288,14 +360,43 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> of integer;</t>
+      <t>;</t>
     </r>
   </si>
   <si>
-    <t>a:of[1..3,10..20] of integer;</t>
-  </si>
-  <si>
-    <t>ab23,be:of[1..3,10..20] of integer;</t>
+    <r>
+      <t>b = (a+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>z</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-215);</t>
+    </r>
+  </si>
+  <si>
+    <t>x := x/y</t>
+  </si>
+  <si>
+    <t>2,P5</t>
+  </si>
+  <si>
+    <t>14,P3</t>
   </si>
 </sst>
 </file>
@@ -311,16 +412,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -351,6 +451,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -364,7 +482,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -388,6 +506,17 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -668,69 +797,70 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q34"/>
+  <dimension ref="A1:R34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="7" max="7" width="10.6640625" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" customWidth="1"/>
     <col min="12" max="12" width="14.109375" customWidth="1"/>
+    <col min="18" max="18" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
-        <v>6</v>
-      </c>
       <c r="G1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" t="s">
         <v>19</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="M1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N1" t="s">
         <v>22</v>
       </c>
-      <c r="K1" t="s">
-        <v>23</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q1" t="s">
         <v>25</v>
       </c>
-      <c r="N1" t="s">
-        <v>24</v>
-      </c>
-      <c r="O1" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
@@ -742,25 +872,25 @@
         <v>4</v>
       </c>
       <c r="E2" s="1">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F2" s="1">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="G2" s="1">
-        <v>8</v>
-      </c>
-      <c r="H2" s="1">
-        <v>11</v>
+        <v>7</v>
+      </c>
+      <c r="H2" s="11">
+        <v>7</v>
       </c>
       <c r="I2" s="1">
         <v>1</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="K2" s="1">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="L2" s="1">
         <v>11</v>
@@ -768,113 +898,119 @@
       <c r="M2" s="1">
         <v>11</v>
       </c>
-      <c r="N2" t="s">
-        <v>28</v>
-      </c>
-      <c r="O2" s="1">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N2">
+        <v>11</v>
+      </c>
+      <c r="O2" s="11">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" s="9">
         <v>1</v>
       </c>
       <c r="C3" s="9">
-        <v>1</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>29</v>
+        <v>2</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>78</v>
       </c>
       <c r="I3" s="1">
         <v>1</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K3" s="1">
-        <v>10</v>
+        <v>0</v>
+      </c>
+      <c r="K3" s="11" t="s">
+        <v>92</v>
       </c>
       <c r="L3" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>1</v>
+        <v>51</v>
+      </c>
+      <c r="M3" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="N3" s="11" t="s">
+        <v>80</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+      <c r="R3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1">
         <v>2</v>
       </c>
-      <c r="C4" s="1">
-        <v>1</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>29</v>
+      <c r="C4" s="11">
+        <v>2</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>78</v>
       </c>
       <c r="I4" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K4" s="1">
-        <v>10</v>
+        <v>0</v>
+      </c>
+      <c r="K4" s="11" t="s">
+        <v>92</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>1</v>
+        <v>51</v>
+      </c>
+      <c r="M4" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="N4" s="11" t="s">
+        <v>80</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+      <c r="R4" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5" s="1">
         <v>3</v>
@@ -882,93 +1018,93 @@
       <c r="D5" s="1">
         <v>4</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>38</v>
+      <c r="E5" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>79</v>
       </c>
       <c r="I5" s="1">
         <v>5</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>41</v>
+        <v>0</v>
+      </c>
+      <c r="K5" s="11" t="s">
+        <v>93</v>
       </c>
       <c r="L5" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>1</v>
+        <v>34</v>
+      </c>
+      <c r="M5" s="11" t="s">
+        <v>84</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="O5" s="11" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" s="1">
         <v>4</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E6" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>38</v>
+      <c r="F6" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>79</v>
       </c>
       <c r="I6" s="1">
         <v>6</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>41</v>
+        <v>0</v>
+      </c>
+      <c r="K6" s="11" t="s">
+        <v>93</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>1</v>
+        <v>34</v>
+      </c>
+      <c r="M6" s="11" t="s">
+        <v>84</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="O6" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="O6" s="11" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" s="1">
         <v>5</v>
@@ -976,186 +1112,189 @@
       <c r="D7" s="1">
         <v>6</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>38</v>
+      <c r="E7" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>79</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>41</v>
+        <v>0</v>
+      </c>
+      <c r="K7" s="11" t="s">
+        <v>93</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>1</v>
+        <v>34</v>
+      </c>
+      <c r="M7" s="11" t="s">
+        <v>84</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="O7" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="O7" s="11" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8" s="1">
         <v>6</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>38</v>
+        <v>0</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>79</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>41</v>
+        <v>0</v>
+      </c>
+      <c r="K8" s="11" t="s">
+        <v>93</v>
       </c>
       <c r="L8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M8" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O8" s="11" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J9" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="M8" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="N8" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="O8" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="K9" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="N9" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="O9" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>14</v>
-      </c>
       <c r="B10" s="1" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>44</v>
+        <v>37</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>85</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>47</v>
+        <v>39</v>
+      </c>
+      <c r="K10" s="11" t="s">
+        <v>0</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R10" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11" s="1">
         <v>9</v>
@@ -1182,7 +1321,7 @@
         <v>9</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="K11" s="1">
         <v>9</v>
@@ -1190,20 +1329,23 @@
       <c r="L11" s="1">
         <v>9</v>
       </c>
-      <c r="M11" s="1">
-        <v>9</v>
+      <c r="M11" s="11" t="s">
+        <v>0</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O11" s="1">
         <v>9</v>
       </c>
       <c r="P11" s="8"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12" s="1">
         <v>10</v>
@@ -1238,297 +1380,379 @@
       <c r="L12" s="1">
         <v>10</v>
       </c>
-      <c r="M12" s="1">
-        <v>10</v>
-      </c>
-      <c r="N12" s="1">
-        <v>10</v>
+      <c r="M12" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="N12" s="11" t="s">
+        <v>41</v>
       </c>
       <c r="O12" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R12" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B13" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="D13" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J13" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="K13" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="L13" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N13" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="O13" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="R13" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H14" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R14" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H15" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R15" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I13" s="1" t="s">
+      <c r="C16" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="J13" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="L13" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="M13" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="N13" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="O13" s="10" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="D16" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L16" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="H14" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="L14" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="M14" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="N14" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="O14" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>62</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="H15" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="L15" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="M15" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="N15" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="O15" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>63</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K16" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="L16" s="9" t="s">
-        <v>69</v>
-      </c>
       <c r="M16" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="R16" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17">
         <v>4</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M17" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="N17" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="G17" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="L17" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="M17" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="N17" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="O17" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="E19" t="s">
-        <v>74</v>
-      </c>
-      <c r="O19" s="1" t="s">
-        <v>60</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A18" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="H18" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="I18" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="J18" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="K18" s="14">
+        <v>10</v>
+      </c>
+      <c r="L18" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="M18" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="N18" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="O18" s="11" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="E20" s="4" t="s">
-        <v>75</v>
+      <c r="E20" s="4"/>
+      <c r="G20" t="s">
+        <v>66</v>
+      </c>
+      <c r="O20" s="1" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
+        <v>59</v>
+      </c>
+      <c r="D21" t="s">
+        <v>64</v>
+      </c>
+      <c r="G21" t="s">
         <v>67</v>
       </c>
-      <c r="D21" t="s">
-        <v>72</v>
-      </c>
-      <c r="E21" t="s">
-        <v>76</v>
-      </c>
       <c r="P21" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
+        <v>60</v>
+      </c>
+      <c r="G22" t="s">
         <v>68</v>
       </c>
       <c r="P22" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="G23" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="D24" t="s">
+        <v>100</v>
+      </c>
+      <c r="E24" t="s">
+        <v>14</v>
+      </c>
+      <c r="G24" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="G25" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="E24" t="s">
-        <v>15</v>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="G26" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="M27" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="N27">
         <v>0</v>
@@ -1536,10 +1760,10 @@
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D28" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="N28" s="5">
         <v>1</v>
@@ -1553,50 +1777,50 @@
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B29">
         <v>2488</v>
       </c>
       <c r="N29" s="5" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="N30" s="4" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="N31" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="N32" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
without round on =
</commit_message>
<xml_diff>
--- a/Interpreter/Interpreter/Лист Microsoft Excel.xlsx
+++ b/Interpreter/Interpreter/Лист Microsoft Excel.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05295A4E-9031-4A60-A2A6-A2B1FC751C96}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="109">
   <si>
     <t>F</t>
   </si>
@@ -250,9 +251,6 @@
   </si>
   <si>
     <t>13,P3</t>
-  </si>
-  <si>
-    <t>операция +-</t>
   </si>
   <si>
     <t>7,P2</t>
@@ -398,11 +396,32 @@
   <si>
     <t>14,P3</t>
   </si>
+  <si>
+    <t xml:space="preserve"> -</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +</t>
+  </si>
+  <si>
+    <t>операция *</t>
+  </si>
+  <si>
+    <t>17,P2</t>
+  </si>
+  <si>
+    <t>18,P2</t>
+  </si>
+  <si>
+    <t>числа с плав точкой</t>
+  </si>
+  <si>
+    <t>числа с плав т и е</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -796,22 +815,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R34"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:T34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N22" sqref="N22"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" customWidth="1"/>
-    <col min="12" max="12" width="14.109375" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" customWidth="1"/>
+    <col min="12" max="12" width="14.140625" customWidth="1"/>
     <col min="18" max="18" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>2</v>
       </c>
@@ -828,7 +847,7 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>77</v>
+        <v>104</v>
       </c>
       <c r="H1" t="s">
         <v>18</v>
@@ -854,11 +873,17 @@
       <c r="O1" t="s">
         <v>46</v>
       </c>
+      <c r="P1" t="s">
+        <v>102</v>
+      </c>
       <c r="Q1" t="s">
+        <v>103</v>
+      </c>
+      <c r="S1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>44</v>
       </c>
@@ -904,8 +929,14 @@
       <c r="O2" s="11">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="P2" s="1">
+        <v>7</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -916,7 +947,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E3" s="11" t="s">
         <v>74</v>
@@ -925,10 +956,10 @@
         <v>75</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I3" s="1">
         <v>1</v>
@@ -937,25 +968,31 @@
         <v>0</v>
       </c>
       <c r="K3" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L3" s="9" t="s">
         <v>51</v>
       </c>
       <c r="M3" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="N3" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="R3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="P3" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q3" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="T3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -966,7 +1003,7 @@
         <v>2</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>74</v>
@@ -975,10 +1012,10 @@
         <v>75</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I4" s="1">
         <v>2</v>
@@ -987,25 +1024,31 @@
         <v>0</v>
       </c>
       <c r="K4" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>51</v>
       </c>
       <c r="M4" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="N4" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="R4" s="4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="P4" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q4" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="T4" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1025,10 +1068,10 @@
         <v>76</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I5" s="1">
         <v>5</v>
@@ -1037,22 +1080,22 @@
         <v>0</v>
       </c>
       <c r="K5" s="11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="L5" s="9" t="s">
         <v>34</v>
       </c>
       <c r="M5" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="N5" s="1" t="s">
         <v>0</v>
       </c>
       <c r="O5" s="11" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -1072,10 +1115,10 @@
         <v>76</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H6" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I6" s="1">
         <v>6</v>
@@ -1084,22 +1127,22 @@
         <v>0</v>
       </c>
       <c r="K6" s="11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="L6" s="1" t="s">
         <v>34</v>
       </c>
       <c r="M6" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="N6" s="1" t="s">
         <v>0</v>
       </c>
       <c r="O6" s="11" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -1119,10 +1162,10 @@
         <v>76</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>0</v>
@@ -1131,22 +1174,22 @@
         <v>0</v>
       </c>
       <c r="K7" s="11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="L7" s="1" t="s">
         <v>34</v>
       </c>
       <c r="M7" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="N7" s="1" t="s">
         <v>0</v>
       </c>
       <c r="O7" s="11" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -1166,10 +1209,10 @@
         <v>76</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>0</v>
@@ -1178,22 +1221,22 @@
         <v>0</v>
       </c>
       <c r="K8" s="11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>34</v>
       </c>
       <c r="M8" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="N8" s="1" t="s">
         <v>0</v>
       </c>
       <c r="O8" s="11" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -1204,7 +1247,7 @@
         <v>37</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>0</v>
@@ -1240,7 +1283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -1251,7 +1294,7 @@
         <v>37</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>0</v>
@@ -1287,12 +1330,12 @@
         <v>0</v>
       </c>
       <c r="P10" s="1"/>
-      <c r="Q10" s="1"/>
-      <c r="R10" t="s">
+      <c r="S10" s="1"/>
+      <c r="T10" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -1339,11 +1382,11 @@
         <v>9</v>
       </c>
       <c r="P11" s="8"/>
-      <c r="R11" t="s">
+      <c r="T11" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -1389,11 +1432,11 @@
       <c r="O12" s="1">
         <v>10</v>
       </c>
-      <c r="R12" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -1404,28 +1447,28 @@
         <v>50</v>
       </c>
       <c r="D13" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="E13" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="F13" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="F13" s="11" t="s">
+      <c r="G13" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="G13" s="11" t="s">
-        <v>89</v>
-      </c>
       <c r="H13" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>42</v>
       </c>
       <c r="J13" s="11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K13" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="L13" s="9" t="s">
         <v>1</v>
@@ -1439,11 +1482,11 @@
       <c r="O13" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="R13" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T13" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>53</v>
       </c>
@@ -1454,7 +1497,7 @@
         <v>37</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>0</v>
@@ -1489,11 +1532,11 @@
       <c r="O14" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="R14" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T14" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>54</v>
       </c>
@@ -1504,7 +1547,7 @@
         <v>37</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>0</v>
@@ -1539,11 +1582,11 @@
       <c r="O15" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="R15" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T15" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>55</v>
       </c>
@@ -1554,7 +1597,7 @@
         <v>50</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>0</v>
@@ -1589,11 +1632,11 @@
       <c r="O16" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="R16" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="T16" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>56</v>
       </c>
@@ -1640,18 +1683,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C18" s="11" t="s">
         <v>37</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E18" s="11" t="s">
         <v>0</v>
@@ -1666,7 +1709,7 @@
         <v>48</v>
       </c>
       <c r="I18" s="11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J18" s="11" t="s">
         <v>0</v>
@@ -1687,7 +1730,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>108</v>
+      </c>
       <c r="E20" s="4"/>
       <c r="G20" t="s">
         <v>66</v>
@@ -1696,7 +1747,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>59</v>
       </c>
@@ -1710,7 +1761,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>60</v>
       </c>
@@ -1721,14 +1772,14 @@
         <v>63</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="G23" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D24" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E24" t="s">
         <v>14</v>
@@ -1737,17 +1788,17 @@
         <v>70</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="G25" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="G26" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -1758,7 +1809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -1775,7 +1826,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -1786,7 +1837,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -1794,7 +1845,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -1805,7 +1856,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -1813,12 +1864,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>33</v>
       </c>

</xml_diff>